<commit_message>
Adding the onset qu to the test config
</commit_message>
<xml_diff>
--- a/triple-vietnamese.xlsx
+++ b/triple-vietnamese.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="218">
   <si>
     <t xml:space="preserve">bcd</t>
   </si>
@@ -28,16 +28,19 @@
     <t xml:space="preserve">aáàảãạ</t>
   </si>
   <si>
+    <t xml:space="preserve">qu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k/c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t</t>
+  </si>
+  <si>
     <t xml:space="preserve">ch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k/c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t</t>
   </si>
   <si>
     <t xml:space="preserve">ng(h)</t>
@@ -681,7 +684,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -724,6 +727,12 @@
       <name val="Noto Sans"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Noto Sans"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="12"/>
@@ -898,7 +907,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -927,6 +936,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -951,19 +964,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -999,11 +1012,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="16" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="16" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="14" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="14" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1322,7 +1335,7 @@
     </row>
     <row r="2" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6"/>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1334,178 +1347,180 @@
       <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="G2" s="2"/>
       <c r="H2" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="3"/>
-      <c r="N2" s="7"/>
+      <c r="N2" s="8"/>
       <c r="O2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="Q2" s="8" t="s">
         <v>13</v>
       </c>
+      <c r="R2" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="S2" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="U2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="U2" s="8" t="s">
         <v>17</v>
       </c>
+      <c r="V2" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="W2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y2" s="7"/>
+        <v>20</v>
+      </c>
+      <c r="Y2" s="8"/>
       <c r="Z2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6"/>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="6"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="7"/>
+      <c r="N3" s="8"/>
       <c r="O3" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="Q3" s="8" t="s">
         <v>32</v>
       </c>
+      <c r="R3" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="S3" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="U3" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="V3" s="7" t="s">
+      <c r="U3" s="8" t="s">
         <v>36</v>
       </c>
+      <c r="V3" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="W3" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y3" s="7"/>
+        <v>39</v>
+      </c>
+      <c r="Y3" s="8"/>
       <c r="Z3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
       <c r="B4" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="6"/>
       <c r="M4" s="3"/>
-      <c r="N4" s="7"/>
+      <c r="N4" s="8"/>
       <c r="O4" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q4" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="R4" s="7" t="s">
+      <c r="Q4" s="8" t="s">
         <v>48</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
-      <c r="U4" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="V4" s="7" t="s">
+      <c r="U4" s="8" t="s">
         <v>50</v>
       </c>
+      <c r="V4" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="W4" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="X4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y4" s="7"/>
+        <v>53</v>
+      </c>
+      <c r="Y4" s="8"/>
       <c r="Z4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1537,915 +1552,915 @@
       <c r="Z5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="10"/>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="10"/>
+      <c r="A6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
       <c r="Z6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11"/>
-      <c r="B7" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="8" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="D7" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="E7" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="11" t="s">
+      <c r="F7" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="G7" s="9"/>
+      <c r="H7" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="I7" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="J7" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="K7" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="M7" s="9"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="13" t="s">
+      <c r="L7" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="Q7" s="14" t="s">
+      <c r="M7" s="10"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="R7" s="14" t="s">
+      <c r="Q7" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="12"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="10"/>
-      <c r="Y7" s="12"/>
+      <c r="R7" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="14"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="13"/>
       <c r="Z7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11"/>
-      <c r="B8" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="8" t="s">
+      <c r="A8" s="12"/>
+      <c r="B8" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="8" t="s">
+      <c r="D8" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="E8" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="G8" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="H8" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="I8" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="J8" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="L8" s="11" t="s">
+      <c r="K8" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="M8" s="9"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="16" t="s">
+      <c r="L8" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="P8" s="13" t="s">
+      <c r="M8" s="10"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="Q8" s="14" t="s">
+      <c r="P8" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="R8" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="14" t="s">
+      <c r="Q8" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="V8" s="14" t="s">
+      <c r="R8" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="W8" s="13" t="s">
+      <c r="V8" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="X8" s="16" t="s">
+      <c r="W8" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="Y8" s="12"/>
+      <c r="X8" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y8" s="13"/>
       <c r="Z8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11"/>
-      <c r="B9" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="11" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="D9" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="11" t="s">
+      <c r="E9" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="I9" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="J9" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="L9" s="11"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="13" t="s">
+      <c r="K9" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="Q9" s="14" t="s">
+      <c r="L9" s="12"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="R9" s="14" t="s">
+      <c r="Q9" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="12"/>
-      <c r="W9" s="10"/>
-      <c r="X9" s="10"/>
-      <c r="Y9" s="12"/>
+      <c r="R9" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="13"/>
       <c r="Z9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9"/>
-      <c r="Y10" s="9"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
       <c r="Z10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="18"/>
+      <c r="A11" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19"/>
+      <c r="X11" s="19"/>
+      <c r="Y11" s="19"/>
       <c r="Z11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="19"/>
-      <c r="B12" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="C12" s="20" t="s">
+      <c r="A12" s="20"/>
+      <c r="B12" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="C12" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="D12" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="E12" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="F12" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="G12" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="H12" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="J12" s="20" t="s">
+      <c r="I12" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="K12" s="20" t="s">
+      <c r="J12" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="L12" s="19"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="22" t="s">
+      <c r="K12" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="P12" s="22" t="s">
+      <c r="L12" s="20"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="Q12" s="21" t="s">
+      <c r="P12" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="R12" s="21" t="s">
+      <c r="Q12" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="S12" s="22" t="s">
+      <c r="R12" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="T12" s="22" t="s">
+      <c r="S12" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="U12" s="21" t="s">
+      <c r="T12" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="V12" s="21" t="s">
+      <c r="U12" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="W12" s="22" t="s">
+      <c r="V12" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="X12" s="22"/>
-      <c r="Y12" s="21"/>
+      <c r="W12" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="X12" s="23"/>
+      <c r="Y12" s="22"/>
       <c r="Z12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="19"/>
-      <c r="B13" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="D13" s="19" t="s">
+      <c r="A13" s="20"/>
+      <c r="B13" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="D13" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="E13" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="F13" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="G13" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="I13" s="19" t="s">
+      <c r="H13" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="J13" s="20" t="s">
+      <c r="I13" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="K13" s="20" t="s">
+      <c r="J13" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="L13" s="19"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="P13" s="22" t="s">
+      <c r="K13" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="Q13" s="21" t="s">
+      <c r="L13" s="20"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="P13" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="R13" s="21" t="s">
+      <c r="Q13" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="S13" s="22" t="s">
+      <c r="R13" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="T13" s="22" t="s">
+      <c r="S13" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="U13" s="21" t="s">
+      <c r="T13" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="V13" s="21" t="s">
+      <c r="U13" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="W13" s="22" t="s">
+      <c r="V13" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="X13" s="22" t="s">
+      <c r="W13" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="Y13" s="21"/>
+      <c r="X13" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y13" s="22"/>
       <c r="Z13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19"/>
-      <c r="B14" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="C14" s="20" t="s">
+      <c r="A14" s="20"/>
+      <c r="B14" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="C14" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="D14" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="E14" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="F14" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="G14" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="I14" s="19" t="s">
+      <c r="H14" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="J14" s="20" t="s">
+      <c r="I14" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="K14" s="20" t="s">
+      <c r="J14" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="L14" s="19"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="22" t="s">
+      <c r="K14" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="P14" s="22" t="s">
+      <c r="L14" s="20"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="Q14" s="21" t="s">
+      <c r="P14" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="R14" s="21" t="s">
+      <c r="Q14" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="S14" s="22" t="s">
+      <c r="R14" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="T14" s="22" t="s">
+      <c r="S14" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="U14" s="21" t="s">
+      <c r="T14" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="V14" s="21" t="s">
+      <c r="U14" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="W14" s="22" t="s">
+      <c r="V14" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="X14" s="22"/>
-      <c r="Y14" s="21"/>
+      <c r="W14" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="X14" s="23"/>
+      <c r="Y14" s="22"/>
       <c r="Z14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="9"/>
-      <c r="U15" s="9"/>
-      <c r="V15" s="9"/>
-      <c r="W15" s="9"/>
-      <c r="X15" s="9"/>
-      <c r="Y15" s="9"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10"/>
       <c r="Z15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="24" t="s">
+      <c r="A16" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="24"/>
-      <c r="U16" s="24"/>
-      <c r="V16" s="24"/>
-      <c r="W16" s="24"/>
-      <c r="X16" s="24"/>
-      <c r="Y16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25"/>
+      <c r="T16" s="25"/>
+      <c r="U16" s="25"/>
+      <c r="V16" s="25"/>
+      <c r="W16" s="25"/>
+      <c r="X16" s="25"/>
+      <c r="Y16" s="25"/>
       <c r="Z16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="25"/>
-      <c r="B17" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="C17" s="26" t="s">
+      <c r="A17" s="26"/>
+      <c r="B17" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="C17" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="D17" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="F17" s="26" t="s">
+      <c r="E17" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="G17" s="26" t="s">
+      <c r="F17" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="H17" s="25" t="s">
+      <c r="G17" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="I17" s="25" t="s">
+      <c r="H17" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="J17" s="26" t="s">
+      <c r="I17" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="K17" s="26" t="s">
+      <c r="J17" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="L17" s="25" t="s">
+      <c r="K17" s="27" t="s">
         <v>161</v>
       </c>
-      <c r="M17" s="9"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="24" t="s">
+      <c r="L17" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="Q17" s="27" t="s">
+      <c r="M17" s="10"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="R17" s="27" t="s">
+      <c r="Q17" s="28" t="s">
         <v>164</v>
       </c>
-      <c r="S17" s="24"/>
-      <c r="T17" s="24"/>
-      <c r="U17" s="27" t="s">
+      <c r="R17" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="V17" s="27" t="s">
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="W17" s="24" t="s">
+      <c r="V17" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="X17" s="24"/>
-      <c r="Y17" s="27"/>
+      <c r="W17" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="X17" s="25"/>
+      <c r="Y17" s="28"/>
       <c r="Z17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="25"/>
-      <c r="B18" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>168</v>
-      </c>
-      <c r="D18" s="25" t="s">
+      <c r="A18" s="26"/>
+      <c r="B18" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="C18" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="D18" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="F18" s="26" t="s">
+      <c r="E18" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="G18" s="26" t="s">
+      <c r="F18" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="H18" s="25" t="s">
+      <c r="G18" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="I18" s="25" t="s">
+      <c r="H18" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="J18" s="26" t="s">
+      <c r="I18" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="K18" s="26" t="s">
+      <c r="J18" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="L18" s="25" t="s">
+      <c r="K18" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="M18" s="9"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="24" t="s">
+      <c r="L18" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="P18" s="24" t="s">
+      <c r="M18" s="10"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="Q18" s="27" t="s">
+      <c r="P18" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="R18" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="S18" s="24"/>
-      <c r="T18" s="24" t="s">
+      <c r="Q18" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="U18" s="27" t="s">
+      <c r="R18" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="S18" s="25"/>
+      <c r="T18" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="V18" s="27" t="s">
+      <c r="U18" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="W18" s="24" t="s">
+      <c r="V18" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="X18" s="24" t="s">
+      <c r="W18" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="Y18" s="27"/>
+      <c r="X18" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y18" s="28"/>
       <c r="Z18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="28"/>
-      <c r="B19" s="26" t="s">
-        <v>186</v>
-      </c>
-      <c r="C19" s="26" t="s">
+      <c r="A19" s="29"/>
+      <c r="B19" s="27" t="s">
         <v>187</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="C19" s="27" t="s">
         <v>188</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="D19" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="E19" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="G19" s="26" t="s">
+      <c r="F19" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="H19" s="25" t="s">
+      <c r="G19" s="27" t="s">
         <v>192</v>
       </c>
-      <c r="I19" s="25" t="s">
+      <c r="H19" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="J19" s="26" t="s">
+      <c r="I19" s="26" t="s">
         <v>194</v>
       </c>
-      <c r="K19" s="26" t="s">
+      <c r="J19" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="L19" s="28"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="27"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24" t="s">
+      <c r="K19" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="Q19" s="27" t="s">
+      <c r="L19" s="29"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="R19" s="27" t="s">
+      <c r="Q19" s="28" t="s">
         <v>198</v>
       </c>
-      <c r="S19" s="24"/>
-      <c r="T19" s="24"/>
-      <c r="U19" s="27" t="s">
+      <c r="R19" s="28" t="s">
         <v>199</v>
       </c>
-      <c r="V19" s="27" t="s">
+      <c r="S19" s="25"/>
+      <c r="T19" s="25"/>
+      <c r="U19" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="W19" s="24" t="s">
+      <c r="V19" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="X19" s="24"/>
-      <c r="Y19" s="27"/>
+      <c r="W19" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="X19" s="25"/>
+      <c r="Y19" s="28"/>
       <c r="Z19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="29"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="29"/>
-      <c r="O20" s="29"/>
-      <c r="P20" s="29"/>
-      <c r="Q20" s="29"/>
-      <c r="R20" s="29"/>
-      <c r="S20" s="29"/>
-      <c r="T20" s="29"/>
-      <c r="U20" s="29"/>
-      <c r="V20" s="29"/>
-      <c r="W20" s="29"/>
-      <c r="X20" s="29"/>
-      <c r="Y20" s="29"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="30"/>
+      <c r="R20" s="30"/>
+      <c r="S20" s="30"/>
+      <c r="T20" s="30"/>
+      <c r="U20" s="30"/>
+      <c r="V20" s="30"/>
+      <c r="W20" s="30"/>
+      <c r="X20" s="30"/>
+      <c r="Y20" s="30"/>
       <c r="Z20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="30" t="s">
-        <v>202</v>
-      </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="29"/>
-      <c r="O21" s="29"/>
-      <c r="P21" s="29"/>
-      <c r="Q21" s="29"/>
-      <c r="R21" s="29"/>
-      <c r="S21" s="29"/>
-      <c r="T21" s="29"/>
-      <c r="U21" s="29"/>
-      <c r="V21" s="29"/>
-      <c r="W21" s="29"/>
-      <c r="X21" s="29"/>
-      <c r="Y21" s="29"/>
+      <c r="A21" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="30"/>
+      <c r="R21" s="30"/>
+      <c r="S21" s="30"/>
+      <c r="T21" s="30"/>
+      <c r="U21" s="30"/>
+      <c r="V21" s="30"/>
+      <c r="W21" s="30"/>
+      <c r="X21" s="30"/>
+      <c r="Y21" s="30"/>
       <c r="Z21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="31"/>
-      <c r="B22" s="30" t="s">
-        <v>203</v>
-      </c>
-      <c r="C22" s="30" t="s">
+      <c r="A22" s="32"/>
+      <c r="B22" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="D22" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="E22" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="30" t="s">
+      <c r="C22" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="G22" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="H22" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="I22" s="31" t="str">
+      <c r="G22" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="H22" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="I22" s="32" t="str">
         <f aca="false">"i"</f>
         <v>i</v>
       </c>
-      <c r="J22" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="K22" s="30" t="s">
+      <c r="J22" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="K22" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="L22" s="31" t="s">
-        <v>205</v>
-      </c>
-      <c r="M22" s="29"/>
-      <c r="N22" s="29"/>
-      <c r="O22" s="29"/>
-      <c r="P22" s="29"/>
-      <c r="Q22" s="29"/>
-      <c r="R22" s="29"/>
-      <c r="S22" s="29"/>
-      <c r="T22" s="29"/>
-      <c r="U22" s="29"/>
-      <c r="V22" s="29"/>
-      <c r="W22" s="29"/>
-      <c r="X22" s="29"/>
-      <c r="Y22" s="29"/>
+      <c r="L22" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="30"/>
+      <c r="P22" s="30"/>
+      <c r="Q22" s="30"/>
+      <c r="R22" s="30"/>
+      <c r="S22" s="30"/>
+      <c r="T22" s="30"/>
+      <c r="U22" s="30"/>
+      <c r="V22" s="30"/>
+      <c r="W22" s="30"/>
+      <c r="X22" s="30"/>
+      <c r="Y22" s="30"/>
       <c r="Z22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="31"/>
-      <c r="B23" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" s="31" t="s">
-        <v>206</v>
-      </c>
-      <c r="F23" s="30" t="s">
+      <c r="A23" s="32"/>
+      <c r="B23" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="32" t="s">
         <v>207</v>
       </c>
-      <c r="G23" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" s="31" t="s">
+      <c r="F23" s="31" t="s">
         <v>208</v>
       </c>
-      <c r="I23" s="31" t="s">
+      <c r="G23" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="J23" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="K23" s="30" t="s">
+      <c r="I23" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="L23" s="31" t="s">
+      <c r="J23" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="K23" s="31" t="s">
         <v>211</v>
       </c>
-      <c r="M23" s="29"/>
-      <c r="N23" s="29"/>
-      <c r="O23" s="29"/>
-      <c r="P23" s="29"/>
-      <c r="Q23" s="29"/>
-      <c r="R23" s="29"/>
-      <c r="S23" s="29"/>
-      <c r="T23" s="29"/>
-      <c r="U23" s="29"/>
-      <c r="V23" s="29"/>
-      <c r="W23" s="29"/>
-      <c r="X23" s="29"/>
-      <c r="Y23" s="29"/>
+      <c r="L23" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="M23" s="30"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="30"/>
+      <c r="R23" s="30"/>
+      <c r="S23" s="30"/>
+      <c r="T23" s="30"/>
+      <c r="U23" s="30"/>
+      <c r="V23" s="30"/>
+      <c r="W23" s="30"/>
+      <c r="X23" s="30"/>
+      <c r="Y23" s="30"/>
       <c r="Z23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="31"/>
-      <c r="B24" s="30" t="s">
-        <v>212</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="31" t="s">
+      <c r="A24" s="32"/>
+      <c r="B24" s="31" t="s">
         <v>213</v>
       </c>
-      <c r="E24" s="31" t="s">
+      <c r="C24" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="E24" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H24" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="I24" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="J24" s="30" t="s">
+      <c r="H24" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="I24" s="32" t="s">
         <v>215</v>
       </c>
-      <c r="K24" s="30" t="s">
+      <c r="J24" s="31" t="s">
         <v>216</v>
       </c>
-      <c r="L24" s="31"/>
-      <c r="M24" s="29"/>
-      <c r="U24" s="29"/>
-      <c r="V24" s="29"/>
-      <c r="W24" s="29"/>
-      <c r="X24" s="29"/>
-      <c r="Y24" s="29"/>
+      <c r="K24" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="L24" s="32"/>
+      <c r="M24" s="30"/>
+      <c r="U24" s="30"/>
+      <c r="V24" s="30"/>
+      <c r="W24" s="30"/>
+      <c r="X24" s="30"/>
+      <c r="Y24" s="30"/>
       <c r="Z24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>